<commit_message>
add part consistency matrix
</commit_message>
<xml_diff>
--- a/data/exerciseData.xlsx
+++ b/data/exerciseData.xlsx
@@ -6,14 +6,16 @@
   </bookViews>
   <sheets>
     <sheet name="preliminaryImpactFactors" sheetId="103" state="visible" r:id="rId1"/>
-    <sheet name="impactMatrix" sheetId="104" state="visible" r:id="rId2"/>
+    <sheet name="impactMatrix" sheetId="106" state="visible" r:id="rId2"/>
+    <sheet name="impactFactorLevels" sheetId="107" state="visible" r:id="rId3"/>
+    <sheet name="impactFactorConsistency" sheetId="108" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="163">
   <si>
     <t>E-Bike price</t>
   </si>
@@ -295,6 +297,216 @@
   </si>
   <si>
     <t xml:space="preserve">integration publ trans</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ImpactFactor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Indicator</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Current_Stat</t>
+  </si>
+  <si>
+    <t xml:space="preserve">trend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">min</t>
+  </si>
+  <si>
+    <t xml:space="preserve">max</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">low, high</t>
+  </si>
+  <si>
+    <t xml:space="preserve">some, everywhere</t>
+  </si>
+  <si>
+    <t xml:space="preserve">none, strict</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF/l</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHF/kwh</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Impact</t>
+  </si>
+  <si>
+    <t xml:space="preserve">km</t>
+  </si>
+  <si>
+    <t xml:space="preserve">value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air pollution_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air pollution_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">air pollution_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attractivity of biking_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attractivity of biking_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">attractivity of biking_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery tech_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery tech_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Battery tech_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bike lanes_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bike lanes_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bike lanes_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">charging infrastructure_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">charging infrastructure_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">charging infrastructure_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commuters willingness_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commuters willingness_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">commuters willingness_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commuting distances_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commuting distances_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Commuting distances_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Bike price_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Bike price_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E-Bike price_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity prize_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity prize_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">electricity prize_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environmental awareness_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environmental awareness_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">environmental awareness_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gasoline price_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gasoline price_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">gasoline price_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integration publ trans_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integration publ trans_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">integration publ trans_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laws and regulations_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laws and regulations_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">laws and regulations_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Bike Price_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Bike Price_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Regular Bike Price_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 25kmh_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 25kmh_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 25kmh_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 45kmh_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 45kmh_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">regulation e-bike 45kmh_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road safety_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road safety_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">road safety_NA2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traffic congestion_NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traffic congestion_NA1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">traffic congestion_NA2</t>
   </si>
 </sst>
 </file>
@@ -1898,4 +2110,3678 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C1" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" t="s">
+        <v>97</v>
+      </c>
+      <c r="E1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F1" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" t="s">
+        <v>101</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" t="s">
+        <v>102</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>90</v>
+      </c>
+      <c r="B6" t="s">
+        <v>103</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>91</v>
+      </c>
+      <c r="B7" t="s">
+        <v>103</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>88</v>
+      </c>
+      <c r="B8" t="s">
+        <v>102</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" t="s">
+        <v>104</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11" t="s">
+        <v>106</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>77</v>
+      </c>
+      <c r="B13" t="s">
+        <v>108</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>93</v>
+      </c>
+      <c r="B14" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B15" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>79</v>
+      </c>
+      <c r="B16" t="s">
+        <v>101</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>80</v>
+      </c>
+      <c r="B17" t="s">
+        <v>101</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18" t="s">
+        <v>101</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>92</v>
+      </c>
+      <c r="B19" t="s">
+        <v>101</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.0"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B1" t="s">
+        <v>109</v>
+      </c>
+      <c r="C1" t="s">
+        <v>110</v>
+      </c>
+      <c r="D1" t="s">
+        <v>111</v>
+      </c>
+      <c r="E1" t="s">
+        <v>112</v>
+      </c>
+      <c r="F1" t="s">
+        <v>113</v>
+      </c>
+      <c r="G1" t="s">
+        <v>114</v>
+      </c>
+      <c r="H1" t="s">
+        <v>115</v>
+      </c>
+      <c r="I1" t="s">
+        <v>116</v>
+      </c>
+      <c r="J1" t="s">
+        <v>117</v>
+      </c>
+      <c r="K1" t="s">
+        <v>118</v>
+      </c>
+      <c r="L1" t="s">
+        <v>119</v>
+      </c>
+      <c r="M1" t="s">
+        <v>120</v>
+      </c>
+      <c r="N1" t="s">
+        <v>121</v>
+      </c>
+      <c r="O1" t="s">
+        <v>122</v>
+      </c>
+      <c r="P1" t="s">
+        <v>123</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>124</v>
+      </c>
+      <c r="R1" t="s">
+        <v>125</v>
+      </c>
+      <c r="S1" t="s">
+        <v>126</v>
+      </c>
+      <c r="T1" t="s">
+        <v>127</v>
+      </c>
+      <c r="U1" t="s">
+        <v>128</v>
+      </c>
+      <c r="V1" t="s">
+        <v>129</v>
+      </c>
+      <c r="W1" t="s">
+        <v>130</v>
+      </c>
+      <c r="X1" t="s">
+        <v>131</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>132</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>133</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>134</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>135</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>136</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>137</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>138</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>139</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>140</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>141</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>142</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>143</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>144</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>145</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>146</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>147</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>148</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>149</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>150</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>151</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>152</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>153</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>154</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>155</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>156</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>157</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>158</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>159</v>
+      </c>
+      <c r="BA1" t="s">
+        <v>160</v>
+      </c>
+      <c r="BB1" t="s">
+        <v>161</v>
+      </c>
+      <c r="BC1" t="s">
+        <v>162</v>
+      </c>
+      <c r="BD1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B2"/>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2"/>
+      <c r="K2"/>
+      <c r="L2"/>
+      <c r="M2"/>
+      <c r="N2"/>
+      <c r="O2"/>
+      <c r="P2"/>
+      <c r="Q2"/>
+      <c r="R2"/>
+      <c r="S2"/>
+      <c r="T2"/>
+      <c r="U2"/>
+      <c r="V2"/>
+      <c r="W2"/>
+      <c r="X2"/>
+      <c r="Y2"/>
+      <c r="Z2"/>
+      <c r="AA2"/>
+      <c r="AB2"/>
+      <c r="AC2"/>
+      <c r="AD2"/>
+      <c r="AE2"/>
+      <c r="AF2"/>
+      <c r="AG2"/>
+      <c r="AH2"/>
+      <c r="AI2"/>
+      <c r="AJ2"/>
+      <c r="AK2"/>
+      <c r="AL2"/>
+      <c r="AM2"/>
+      <c r="AN2"/>
+      <c r="AO2"/>
+      <c r="AP2"/>
+      <c r="AQ2"/>
+      <c r="AR2"/>
+      <c r="AS2"/>
+      <c r="AT2"/>
+      <c r="AU2"/>
+      <c r="AV2"/>
+      <c r="AW2"/>
+      <c r="AX2"/>
+      <c r="AY2"/>
+      <c r="AZ2"/>
+      <c r="BA2"/>
+      <c r="BB2"/>
+      <c r="BC2"/>
+      <c r="BD2"/>
+    </row>
+    <row r="3">
+      <c r="A3" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3"/>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3"/>
+      <c r="K3"/>
+      <c r="L3"/>
+      <c r="M3"/>
+      <c r="N3"/>
+      <c r="O3"/>
+      <c r="P3"/>
+      <c r="Q3"/>
+      <c r="R3"/>
+      <c r="S3"/>
+      <c r="T3"/>
+      <c r="U3"/>
+      <c r="V3"/>
+      <c r="W3"/>
+      <c r="X3"/>
+      <c r="Y3"/>
+      <c r="Z3"/>
+      <c r="AA3"/>
+      <c r="AB3"/>
+      <c r="AC3"/>
+      <c r="AD3"/>
+      <c r="AE3"/>
+      <c r="AF3"/>
+      <c r="AG3"/>
+      <c r="AH3"/>
+      <c r="AI3"/>
+      <c r="AJ3"/>
+      <c r="AK3"/>
+      <c r="AL3"/>
+      <c r="AM3"/>
+      <c r="AN3"/>
+      <c r="AO3"/>
+      <c r="AP3"/>
+      <c r="AQ3"/>
+      <c r="AR3"/>
+      <c r="AS3"/>
+      <c r="AT3"/>
+      <c r="AU3"/>
+      <c r="AV3"/>
+      <c r="AW3"/>
+      <c r="AX3"/>
+      <c r="AY3"/>
+      <c r="AZ3"/>
+      <c r="BA3"/>
+      <c r="BB3"/>
+      <c r="BC3"/>
+      <c r="BD3"/>
+    </row>
+    <row r="4">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4"/>
+      <c r="K4"/>
+      <c r="L4"/>
+      <c r="M4"/>
+      <c r="N4"/>
+      <c r="O4"/>
+      <c r="P4"/>
+      <c r="Q4"/>
+      <c r="R4"/>
+      <c r="S4"/>
+      <c r="T4"/>
+      <c r="U4"/>
+      <c r="V4"/>
+      <c r="W4"/>
+      <c r="X4"/>
+      <c r="Y4"/>
+      <c r="Z4"/>
+      <c r="AA4"/>
+      <c r="AB4"/>
+      <c r="AC4"/>
+      <c r="AD4"/>
+      <c r="AE4"/>
+      <c r="AF4"/>
+      <c r="AG4"/>
+      <c r="AH4"/>
+      <c r="AI4"/>
+      <c r="AJ4"/>
+      <c r="AK4"/>
+      <c r="AL4"/>
+      <c r="AM4"/>
+      <c r="AN4"/>
+      <c r="AO4"/>
+      <c r="AP4"/>
+      <c r="AQ4"/>
+      <c r="AR4"/>
+      <c r="AS4"/>
+      <c r="AT4"/>
+      <c r="AU4"/>
+      <c r="AV4"/>
+      <c r="AW4"/>
+      <c r="AX4"/>
+      <c r="AY4"/>
+      <c r="AZ4"/>
+      <c r="BA4"/>
+      <c r="BB4"/>
+      <c r="BC4"/>
+      <c r="BD4"/>
+    </row>
+    <row r="5">
+      <c r="A5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5"/>
+      <c r="K5"/>
+      <c r="L5"/>
+      <c r="M5"/>
+      <c r="N5"/>
+      <c r="O5"/>
+      <c r="P5"/>
+      <c r="Q5"/>
+      <c r="R5"/>
+      <c r="S5"/>
+      <c r="T5"/>
+      <c r="U5"/>
+      <c r="V5"/>
+      <c r="W5"/>
+      <c r="X5"/>
+      <c r="Y5"/>
+      <c r="Z5"/>
+      <c r="AA5"/>
+      <c r="AB5"/>
+      <c r="AC5"/>
+      <c r="AD5"/>
+      <c r="AE5"/>
+      <c r="AF5"/>
+      <c r="AG5"/>
+      <c r="AH5"/>
+      <c r="AI5"/>
+      <c r="AJ5"/>
+      <c r="AK5"/>
+      <c r="AL5"/>
+      <c r="AM5"/>
+      <c r="AN5"/>
+      <c r="AO5"/>
+      <c r="AP5"/>
+      <c r="AQ5"/>
+      <c r="AR5"/>
+      <c r="AS5"/>
+      <c r="AT5"/>
+      <c r="AU5"/>
+      <c r="AV5"/>
+      <c r="AW5"/>
+      <c r="AX5"/>
+      <c r="AY5"/>
+      <c r="AZ5"/>
+      <c r="BA5"/>
+      <c r="BB5"/>
+      <c r="BC5"/>
+      <c r="BD5"/>
+    </row>
+    <row r="6">
+      <c r="A6" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
+      <c r="Q6"/>
+      <c r="R6"/>
+      <c r="S6"/>
+      <c r="T6"/>
+      <c r="U6"/>
+      <c r="V6"/>
+      <c r="W6"/>
+      <c r="X6"/>
+      <c r="Y6"/>
+      <c r="Z6"/>
+      <c r="AA6"/>
+      <c r="AB6"/>
+      <c r="AC6"/>
+      <c r="AD6"/>
+      <c r="AE6"/>
+      <c r="AF6"/>
+      <c r="AG6"/>
+      <c r="AH6"/>
+      <c r="AI6"/>
+      <c r="AJ6"/>
+      <c r="AK6"/>
+      <c r="AL6"/>
+      <c r="AM6"/>
+      <c r="AN6"/>
+      <c r="AO6"/>
+      <c r="AP6"/>
+      <c r="AQ6"/>
+      <c r="AR6"/>
+      <c r="AS6"/>
+      <c r="AT6"/>
+      <c r="AU6"/>
+      <c r="AV6"/>
+      <c r="AW6"/>
+      <c r="AX6"/>
+      <c r="AY6"/>
+      <c r="AZ6"/>
+      <c r="BA6"/>
+      <c r="BB6"/>
+      <c r="BC6"/>
+      <c r="BD6"/>
+    </row>
+    <row r="7">
+      <c r="A7" t="s">
+        <v>87</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
+      <c r="Q7"/>
+      <c r="R7"/>
+      <c r="S7"/>
+      <c r="T7"/>
+      <c r="U7"/>
+      <c r="V7"/>
+      <c r="W7"/>
+      <c r="X7"/>
+      <c r="Y7"/>
+      <c r="Z7"/>
+      <c r="AA7"/>
+      <c r="AB7"/>
+      <c r="AC7"/>
+      <c r="AD7"/>
+      <c r="AE7"/>
+      <c r="AF7"/>
+      <c r="AG7"/>
+      <c r="AH7"/>
+      <c r="AI7"/>
+      <c r="AJ7"/>
+      <c r="AK7"/>
+      <c r="AL7"/>
+      <c r="AM7"/>
+      <c r="AN7"/>
+      <c r="AO7"/>
+      <c r="AP7"/>
+      <c r="AQ7"/>
+      <c r="AR7"/>
+      <c r="AS7"/>
+      <c r="AT7"/>
+      <c r="AU7"/>
+      <c r="AV7"/>
+      <c r="AW7"/>
+      <c r="AX7"/>
+      <c r="AY7"/>
+      <c r="AZ7"/>
+      <c r="BA7"/>
+      <c r="BB7"/>
+      <c r="BC7"/>
+      <c r="BD7"/>
+    </row>
+    <row r="8">
+      <c r="A8" t="s">
+        <v>84</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8"/>
+      <c r="K8"/>
+      <c r="L8"/>
+      <c r="M8"/>
+      <c r="N8"/>
+      <c r="O8"/>
+      <c r="P8"/>
+      <c r="Q8"/>
+      <c r="R8"/>
+      <c r="S8"/>
+      <c r="T8"/>
+      <c r="U8"/>
+      <c r="V8"/>
+      <c r="W8"/>
+      <c r="X8"/>
+      <c r="Y8"/>
+      <c r="Z8"/>
+      <c r="AA8"/>
+      <c r="AB8"/>
+      <c r="AC8"/>
+      <c r="AD8"/>
+      <c r="AE8"/>
+      <c r="AF8"/>
+      <c r="AG8"/>
+      <c r="AH8"/>
+      <c r="AI8"/>
+      <c r="AJ8"/>
+      <c r="AK8"/>
+      <c r="AL8"/>
+      <c r="AM8"/>
+      <c r="AN8"/>
+      <c r="AO8"/>
+      <c r="AP8"/>
+      <c r="AQ8"/>
+      <c r="AR8"/>
+      <c r="AS8"/>
+      <c r="AT8"/>
+      <c r="AU8"/>
+      <c r="AV8"/>
+      <c r="AW8"/>
+      <c r="AX8"/>
+      <c r="AY8"/>
+      <c r="AZ8"/>
+      <c r="BA8"/>
+      <c r="BB8"/>
+      <c r="BC8"/>
+      <c r="BD8"/>
+    </row>
+    <row r="9">
+      <c r="A9" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9"/>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9"/>
+      <c r="K9"/>
+      <c r="L9"/>
+      <c r="M9"/>
+      <c r="N9"/>
+      <c r="O9"/>
+      <c r="P9"/>
+      <c r="Q9"/>
+      <c r="R9"/>
+      <c r="S9"/>
+      <c r="T9"/>
+      <c r="U9"/>
+      <c r="V9"/>
+      <c r="W9"/>
+      <c r="X9"/>
+      <c r="Y9"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
+      <c r="AK9"/>
+      <c r="AL9"/>
+      <c r="AM9"/>
+      <c r="AN9"/>
+      <c r="AO9"/>
+      <c r="AP9"/>
+      <c r="AQ9"/>
+      <c r="AR9"/>
+      <c r="AS9"/>
+      <c r="AT9"/>
+      <c r="AU9"/>
+      <c r="AV9"/>
+      <c r="AW9"/>
+      <c r="AX9"/>
+      <c r="AY9"/>
+      <c r="AZ9"/>
+      <c r="BA9"/>
+      <c r="BB9"/>
+      <c r="BC9"/>
+      <c r="BD9"/>
+    </row>
+    <row r="10">
+      <c r="A10" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10"/>
+      <c r="K10"/>
+      <c r="L10"/>
+      <c r="M10"/>
+      <c r="N10"/>
+      <c r="O10"/>
+      <c r="P10"/>
+      <c r="Q10"/>
+      <c r="R10"/>
+      <c r="S10"/>
+      <c r="T10"/>
+      <c r="U10"/>
+      <c r="V10"/>
+      <c r="W10"/>
+      <c r="X10"/>
+      <c r="Y10"/>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
+      <c r="AK10"/>
+      <c r="AL10"/>
+      <c r="AM10"/>
+      <c r="AN10"/>
+      <c r="AO10"/>
+      <c r="AP10"/>
+      <c r="AQ10"/>
+      <c r="AR10"/>
+      <c r="AS10"/>
+      <c r="AT10"/>
+      <c r="AU10"/>
+      <c r="AV10"/>
+      <c r="AW10"/>
+      <c r="AX10"/>
+      <c r="AY10"/>
+      <c r="AZ10"/>
+      <c r="BA10"/>
+      <c r="BB10"/>
+      <c r="BC10"/>
+      <c r="BD10"/>
+    </row>
+    <row r="11">
+      <c r="A11" t="s">
+        <v>81</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11"/>
+      <c r="K11"/>
+      <c r="L11"/>
+      <c r="M11"/>
+      <c r="N11"/>
+      <c r="O11"/>
+      <c r="P11"/>
+      <c r="Q11"/>
+      <c r="R11"/>
+      <c r="S11"/>
+      <c r="T11"/>
+      <c r="U11"/>
+      <c r="V11"/>
+      <c r="W11"/>
+      <c r="X11"/>
+      <c r="Y11"/>
+      <c r="Z11"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11"/>
+      <c r="AK11"/>
+      <c r="AL11"/>
+      <c r="AM11"/>
+      <c r="AN11"/>
+      <c r="AO11"/>
+      <c r="AP11"/>
+      <c r="AQ11"/>
+      <c r="AR11"/>
+      <c r="AS11"/>
+      <c r="AT11"/>
+      <c r="AU11"/>
+      <c r="AV11"/>
+      <c r="AW11"/>
+      <c r="AX11"/>
+      <c r="AY11"/>
+      <c r="AZ11"/>
+      <c r="BA11"/>
+      <c r="BB11"/>
+      <c r="BC11"/>
+      <c r="BD11"/>
+    </row>
+    <row r="12">
+      <c r="A12" t="s">
+        <v>81</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12"/>
+      <c r="K12"/>
+      <c r="L12"/>
+      <c r="M12"/>
+      <c r="N12"/>
+      <c r="O12"/>
+      <c r="P12"/>
+      <c r="Q12"/>
+      <c r="R12"/>
+      <c r="S12"/>
+      <c r="T12"/>
+      <c r="U12"/>
+      <c r="V12"/>
+      <c r="W12"/>
+      <c r="X12"/>
+      <c r="Y12"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
+      <c r="AK12"/>
+      <c r="AL12"/>
+      <c r="AM12"/>
+      <c r="AN12"/>
+      <c r="AO12"/>
+      <c r="AP12"/>
+      <c r="AQ12"/>
+      <c r="AR12"/>
+      <c r="AS12"/>
+      <c r="AT12"/>
+      <c r="AU12"/>
+      <c r="AV12"/>
+      <c r="AW12"/>
+      <c r="AX12"/>
+      <c r="AY12"/>
+      <c r="AZ12"/>
+      <c r="BA12"/>
+      <c r="BB12"/>
+      <c r="BC12"/>
+      <c r="BD12"/>
+    </row>
+    <row r="13">
+      <c r="A13" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13"/>
+      <c r="K13"/>
+      <c r="L13"/>
+      <c r="M13"/>
+      <c r="N13"/>
+      <c r="O13"/>
+      <c r="P13"/>
+      <c r="Q13"/>
+      <c r="R13"/>
+      <c r="S13"/>
+      <c r="T13"/>
+      <c r="U13"/>
+      <c r="V13"/>
+      <c r="W13"/>
+      <c r="X13"/>
+      <c r="Y13"/>
+      <c r="Z13"/>
+      <c r="AA13"/>
+      <c r="AB13"/>
+      <c r="AC13"/>
+      <c r="AD13"/>
+      <c r="AE13"/>
+      <c r="AF13"/>
+      <c r="AG13"/>
+      <c r="AH13"/>
+      <c r="AI13"/>
+      <c r="AJ13"/>
+      <c r="AK13"/>
+      <c r="AL13"/>
+      <c r="AM13"/>
+      <c r="AN13"/>
+      <c r="AO13"/>
+      <c r="AP13"/>
+      <c r="AQ13"/>
+      <c r="AR13"/>
+      <c r="AS13"/>
+      <c r="AT13"/>
+      <c r="AU13"/>
+      <c r="AV13"/>
+      <c r="AW13"/>
+      <c r="AX13"/>
+      <c r="AY13"/>
+      <c r="AZ13"/>
+      <c r="BA13"/>
+      <c r="BB13"/>
+      <c r="BC13"/>
+      <c r="BD13"/>
+    </row>
+    <row r="14">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14"/>
+      <c r="K14"/>
+      <c r="L14"/>
+      <c r="M14"/>
+      <c r="N14"/>
+      <c r="O14"/>
+      <c r="P14"/>
+      <c r="Q14"/>
+      <c r="R14"/>
+      <c r="S14"/>
+      <c r="T14"/>
+      <c r="U14"/>
+      <c r="V14"/>
+      <c r="W14"/>
+      <c r="X14"/>
+      <c r="Y14"/>
+      <c r="Z14"/>
+      <c r="AA14"/>
+      <c r="AB14"/>
+      <c r="AC14"/>
+      <c r="AD14"/>
+      <c r="AE14"/>
+      <c r="AF14"/>
+      <c r="AG14"/>
+      <c r="AH14"/>
+      <c r="AI14"/>
+      <c r="AJ14"/>
+      <c r="AK14"/>
+      <c r="AL14"/>
+      <c r="AM14"/>
+      <c r="AN14"/>
+      <c r="AO14"/>
+      <c r="AP14"/>
+      <c r="AQ14"/>
+      <c r="AR14"/>
+      <c r="AS14"/>
+      <c r="AT14"/>
+      <c r="AU14"/>
+      <c r="AV14"/>
+      <c r="AW14"/>
+      <c r="AX14"/>
+      <c r="AY14"/>
+      <c r="AZ14"/>
+      <c r="BA14"/>
+      <c r="BB14"/>
+      <c r="BC14"/>
+      <c r="BD14"/>
+    </row>
+    <row r="15">
+      <c r="A15" t="s">
+        <v>88</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15"/>
+      <c r="K15"/>
+      <c r="L15"/>
+      <c r="M15"/>
+      <c r="N15"/>
+      <c r="O15"/>
+      <c r="P15"/>
+      <c r="Q15"/>
+      <c r="R15"/>
+      <c r="S15"/>
+      <c r="T15"/>
+      <c r="U15"/>
+      <c r="V15"/>
+      <c r="W15"/>
+      <c r="X15"/>
+      <c r="Y15"/>
+      <c r="Z15"/>
+      <c r="AA15"/>
+      <c r="AB15"/>
+      <c r="AC15"/>
+      <c r="AD15"/>
+      <c r="AE15"/>
+      <c r="AF15"/>
+      <c r="AG15"/>
+      <c r="AH15"/>
+      <c r="AI15"/>
+      <c r="AJ15"/>
+      <c r="AK15"/>
+      <c r="AL15"/>
+      <c r="AM15"/>
+      <c r="AN15"/>
+      <c r="AO15"/>
+      <c r="AP15"/>
+      <c r="AQ15"/>
+      <c r="AR15"/>
+      <c r="AS15"/>
+      <c r="AT15"/>
+      <c r="AU15"/>
+      <c r="AV15"/>
+      <c r="AW15"/>
+      <c r="AX15"/>
+      <c r="AY15"/>
+      <c r="AZ15"/>
+      <c r="BA15"/>
+      <c r="BB15"/>
+      <c r="BC15"/>
+      <c r="BD15"/>
+    </row>
+    <row r="16">
+      <c r="A16" t="s">
+        <v>88</v>
+      </c>
+      <c r="B16"/>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16"/>
+      <c r="K16"/>
+      <c r="L16"/>
+      <c r="M16"/>
+      <c r="N16"/>
+      <c r="O16"/>
+      <c r="P16"/>
+      <c r="Q16"/>
+      <c r="R16"/>
+      <c r="S16"/>
+      <c r="T16"/>
+      <c r="U16"/>
+      <c r="V16"/>
+      <c r="W16"/>
+      <c r="X16"/>
+      <c r="Y16"/>
+      <c r="Z16"/>
+      <c r="AA16"/>
+      <c r="AB16"/>
+      <c r="AC16"/>
+      <c r="AD16"/>
+      <c r="AE16"/>
+      <c r="AF16"/>
+      <c r="AG16"/>
+      <c r="AH16"/>
+      <c r="AI16"/>
+      <c r="AJ16"/>
+      <c r="AK16"/>
+      <c r="AL16"/>
+      <c r="AM16"/>
+      <c r="AN16"/>
+      <c r="AO16"/>
+      <c r="AP16"/>
+      <c r="AQ16"/>
+      <c r="AR16"/>
+      <c r="AS16"/>
+      <c r="AT16"/>
+      <c r="AU16"/>
+      <c r="AV16"/>
+      <c r="AW16"/>
+      <c r="AX16"/>
+      <c r="AY16"/>
+      <c r="AZ16"/>
+      <c r="BA16"/>
+      <c r="BB16"/>
+      <c r="BC16"/>
+      <c r="BD16"/>
+    </row>
+    <row r="17">
+      <c r="A17" t="s">
+        <v>89</v>
+      </c>
+      <c r="B17"/>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17"/>
+      <c r="K17"/>
+      <c r="L17"/>
+      <c r="M17"/>
+      <c r="N17"/>
+      <c r="O17"/>
+      <c r="P17"/>
+      <c r="Q17"/>
+      <c r="R17"/>
+      <c r="S17"/>
+      <c r="T17"/>
+      <c r="U17"/>
+      <c r="V17"/>
+      <c r="W17"/>
+      <c r="X17"/>
+      <c r="Y17"/>
+      <c r="Z17"/>
+      <c r="AA17"/>
+      <c r="AB17"/>
+      <c r="AC17"/>
+      <c r="AD17"/>
+      <c r="AE17"/>
+      <c r="AF17"/>
+      <c r="AG17"/>
+      <c r="AH17"/>
+      <c r="AI17"/>
+      <c r="AJ17"/>
+      <c r="AK17"/>
+      <c r="AL17"/>
+      <c r="AM17"/>
+      <c r="AN17"/>
+      <c r="AO17"/>
+      <c r="AP17"/>
+      <c r="AQ17"/>
+      <c r="AR17"/>
+      <c r="AS17"/>
+      <c r="AT17"/>
+      <c r="AU17"/>
+      <c r="AV17"/>
+      <c r="AW17"/>
+      <c r="AX17"/>
+      <c r="AY17"/>
+      <c r="AZ17"/>
+      <c r="BA17"/>
+      <c r="BB17"/>
+      <c r="BC17"/>
+      <c r="BD17"/>
+    </row>
+    <row r="18">
+      <c r="A18" t="s">
+        <v>89</v>
+      </c>
+      <c r="B18"/>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18"/>
+      <c r="K18"/>
+      <c r="L18"/>
+      <c r="M18"/>
+      <c r="N18"/>
+      <c r="O18"/>
+      <c r="P18"/>
+      <c r="Q18"/>
+      <c r="R18"/>
+      <c r="S18"/>
+      <c r="T18"/>
+      <c r="U18"/>
+      <c r="V18"/>
+      <c r="W18"/>
+      <c r="X18"/>
+      <c r="Y18"/>
+      <c r="Z18"/>
+      <c r="AA18"/>
+      <c r="AB18"/>
+      <c r="AC18"/>
+      <c r="AD18"/>
+      <c r="AE18"/>
+      <c r="AF18"/>
+      <c r="AG18"/>
+      <c r="AH18"/>
+      <c r="AI18"/>
+      <c r="AJ18"/>
+      <c r="AK18"/>
+      <c r="AL18"/>
+      <c r="AM18"/>
+      <c r="AN18"/>
+      <c r="AO18"/>
+      <c r="AP18"/>
+      <c r="AQ18"/>
+      <c r="AR18"/>
+      <c r="AS18"/>
+      <c r="AT18"/>
+      <c r="AU18"/>
+      <c r="AV18"/>
+      <c r="AW18"/>
+      <c r="AX18"/>
+      <c r="AY18"/>
+      <c r="AZ18"/>
+      <c r="BA18"/>
+      <c r="BB18"/>
+      <c r="BC18"/>
+      <c r="BD18"/>
+    </row>
+    <row r="19">
+      <c r="A19" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19"/>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
+      <c r="P19"/>
+      <c r="Q19"/>
+      <c r="R19"/>
+      <c r="S19"/>
+      <c r="T19"/>
+      <c r="U19"/>
+      <c r="V19"/>
+      <c r="W19"/>
+      <c r="X19"/>
+      <c r="Y19"/>
+      <c r="Z19"/>
+      <c r="AA19"/>
+      <c r="AB19"/>
+      <c r="AC19"/>
+      <c r="AD19"/>
+      <c r="AE19"/>
+      <c r="AF19"/>
+      <c r="AG19"/>
+      <c r="AH19"/>
+      <c r="AI19"/>
+      <c r="AJ19"/>
+      <c r="AK19"/>
+      <c r="AL19"/>
+      <c r="AM19"/>
+      <c r="AN19"/>
+      <c r="AO19"/>
+      <c r="AP19"/>
+      <c r="AQ19"/>
+      <c r="AR19"/>
+      <c r="AS19"/>
+      <c r="AT19"/>
+      <c r="AU19"/>
+      <c r="AV19"/>
+      <c r="AW19"/>
+      <c r="AX19"/>
+      <c r="AY19"/>
+      <c r="AZ19"/>
+      <c r="BA19"/>
+      <c r="BB19"/>
+      <c r="BC19"/>
+      <c r="BD19"/>
+    </row>
+    <row r="20">
+      <c r="A20" t="s">
+        <v>77</v>
+      </c>
+      <c r="B20"/>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20"/>
+      <c r="K20"/>
+      <c r="L20"/>
+      <c r="M20"/>
+      <c r="N20"/>
+      <c r="O20"/>
+      <c r="P20"/>
+      <c r="Q20"/>
+      <c r="R20"/>
+      <c r="S20"/>
+      <c r="T20"/>
+      <c r="U20"/>
+      <c r="V20"/>
+      <c r="W20"/>
+      <c r="X20"/>
+      <c r="Y20"/>
+      <c r="Z20"/>
+      <c r="AA20"/>
+      <c r="AB20"/>
+      <c r="AC20"/>
+      <c r="AD20"/>
+      <c r="AE20"/>
+      <c r="AF20"/>
+      <c r="AG20"/>
+      <c r="AH20"/>
+      <c r="AI20"/>
+      <c r="AJ20"/>
+      <c r="AK20"/>
+      <c r="AL20"/>
+      <c r="AM20"/>
+      <c r="AN20"/>
+      <c r="AO20"/>
+      <c r="AP20"/>
+      <c r="AQ20"/>
+      <c r="AR20"/>
+      <c r="AS20"/>
+      <c r="AT20"/>
+      <c r="AU20"/>
+      <c r="AV20"/>
+      <c r="AW20"/>
+      <c r="AX20"/>
+      <c r="AY20"/>
+      <c r="AZ20"/>
+      <c r="BA20"/>
+      <c r="BB20"/>
+      <c r="BC20"/>
+      <c r="BD20"/>
+    </row>
+    <row r="21">
+      <c r="A21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B21"/>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21"/>
+      <c r="K21"/>
+      <c r="L21"/>
+      <c r="M21"/>
+      <c r="N21"/>
+      <c r="O21"/>
+      <c r="P21"/>
+      <c r="Q21"/>
+      <c r="R21"/>
+      <c r="S21"/>
+      <c r="T21"/>
+      <c r="U21"/>
+      <c r="V21"/>
+      <c r="W21"/>
+      <c r="X21"/>
+      <c r="Y21"/>
+      <c r="Z21"/>
+      <c r="AA21"/>
+      <c r="AB21"/>
+      <c r="AC21"/>
+      <c r="AD21"/>
+      <c r="AE21"/>
+      <c r="AF21"/>
+      <c r="AG21"/>
+      <c r="AH21"/>
+      <c r="AI21"/>
+      <c r="AJ21"/>
+      <c r="AK21"/>
+      <c r="AL21"/>
+      <c r="AM21"/>
+      <c r="AN21"/>
+      <c r="AO21"/>
+      <c r="AP21"/>
+      <c r="AQ21"/>
+      <c r="AR21"/>
+      <c r="AS21"/>
+      <c r="AT21"/>
+      <c r="AU21"/>
+      <c r="AV21"/>
+      <c r="AW21"/>
+      <c r="AX21"/>
+      <c r="AY21"/>
+      <c r="AZ21"/>
+      <c r="BA21"/>
+      <c r="BB21"/>
+      <c r="BC21"/>
+      <c r="BD21"/>
+    </row>
+    <row r="22">
+      <c r="A22" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22"/>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22"/>
+      <c r="K22"/>
+      <c r="L22"/>
+      <c r="M22"/>
+      <c r="N22"/>
+      <c r="O22"/>
+      <c r="P22"/>
+      <c r="Q22"/>
+      <c r="R22"/>
+      <c r="S22"/>
+      <c r="T22"/>
+      <c r="U22"/>
+      <c r="V22"/>
+      <c r="W22"/>
+      <c r="X22"/>
+      <c r="Y22"/>
+      <c r="Z22"/>
+      <c r="AA22"/>
+      <c r="AB22"/>
+      <c r="AC22"/>
+      <c r="AD22"/>
+      <c r="AE22"/>
+      <c r="AF22"/>
+      <c r="AG22"/>
+      <c r="AH22"/>
+      <c r="AI22"/>
+      <c r="AJ22"/>
+      <c r="AK22"/>
+      <c r="AL22"/>
+      <c r="AM22"/>
+      <c r="AN22"/>
+      <c r="AO22"/>
+      <c r="AP22"/>
+      <c r="AQ22"/>
+      <c r="AR22"/>
+      <c r="AS22"/>
+      <c r="AT22"/>
+      <c r="AU22"/>
+      <c r="AV22"/>
+      <c r="AW22"/>
+      <c r="AX22"/>
+      <c r="AY22"/>
+      <c r="AZ22"/>
+      <c r="BA22"/>
+      <c r="BB22"/>
+      <c r="BC22"/>
+      <c r="BD22"/>
+    </row>
+    <row r="23">
+      <c r="A23" t="s">
+        <v>76</v>
+      </c>
+      <c r="B23"/>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23"/>
+      <c r="K23"/>
+      <c r="L23"/>
+      <c r="M23"/>
+      <c r="N23"/>
+      <c r="O23"/>
+      <c r="P23"/>
+      <c r="Q23"/>
+      <c r="R23"/>
+      <c r="S23"/>
+      <c r="T23"/>
+      <c r="U23"/>
+      <c r="V23"/>
+      <c r="W23"/>
+      <c r="X23"/>
+      <c r="Y23"/>
+      <c r="Z23"/>
+      <c r="AA23"/>
+      <c r="AB23"/>
+      <c r="AC23"/>
+      <c r="AD23"/>
+      <c r="AE23"/>
+      <c r="AF23"/>
+      <c r="AG23"/>
+      <c r="AH23"/>
+      <c r="AI23"/>
+      <c r="AJ23"/>
+      <c r="AK23"/>
+      <c r="AL23"/>
+      <c r="AM23"/>
+      <c r="AN23"/>
+      <c r="AO23"/>
+      <c r="AP23"/>
+      <c r="AQ23"/>
+      <c r="AR23"/>
+      <c r="AS23"/>
+      <c r="AT23"/>
+      <c r="AU23"/>
+      <c r="AV23"/>
+      <c r="AW23"/>
+      <c r="AX23"/>
+      <c r="AY23"/>
+      <c r="AZ23"/>
+      <c r="BA23"/>
+      <c r="BB23"/>
+      <c r="BC23"/>
+      <c r="BD23"/>
+    </row>
+    <row r="24">
+      <c r="A24" t="s">
+        <v>76</v>
+      </c>
+      <c r="B24"/>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24"/>
+      <c r="K24"/>
+      <c r="L24"/>
+      <c r="M24"/>
+      <c r="N24"/>
+      <c r="O24"/>
+      <c r="P24"/>
+      <c r="Q24"/>
+      <c r="R24"/>
+      <c r="S24"/>
+      <c r="T24"/>
+      <c r="U24"/>
+      <c r="V24"/>
+      <c r="W24"/>
+      <c r="X24"/>
+      <c r="Y24"/>
+      <c r="Z24"/>
+      <c r="AA24"/>
+      <c r="AB24"/>
+      <c r="AC24"/>
+      <c r="AD24"/>
+      <c r="AE24"/>
+      <c r="AF24"/>
+      <c r="AG24"/>
+      <c r="AH24"/>
+      <c r="AI24"/>
+      <c r="AJ24"/>
+      <c r="AK24"/>
+      <c r="AL24"/>
+      <c r="AM24"/>
+      <c r="AN24"/>
+      <c r="AO24"/>
+      <c r="AP24"/>
+      <c r="AQ24"/>
+      <c r="AR24"/>
+      <c r="AS24"/>
+      <c r="AT24"/>
+      <c r="AU24"/>
+      <c r="AV24"/>
+      <c r="AW24"/>
+      <c r="AX24"/>
+      <c r="AY24"/>
+      <c r="AZ24"/>
+      <c r="BA24"/>
+      <c r="BB24"/>
+      <c r="BC24"/>
+      <c r="BD24"/>
+    </row>
+    <row r="25">
+      <c r="A25" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25"/>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25"/>
+      <c r="K25"/>
+      <c r="L25"/>
+      <c r="M25"/>
+      <c r="N25"/>
+      <c r="O25"/>
+      <c r="P25"/>
+      <c r="Q25"/>
+      <c r="R25"/>
+      <c r="S25"/>
+      <c r="T25"/>
+      <c r="U25"/>
+      <c r="V25"/>
+      <c r="W25"/>
+      <c r="X25"/>
+      <c r="Y25"/>
+      <c r="Z25"/>
+      <c r="AA25"/>
+      <c r="AB25"/>
+      <c r="AC25"/>
+      <c r="AD25"/>
+      <c r="AE25"/>
+      <c r="AF25"/>
+      <c r="AG25"/>
+      <c r="AH25"/>
+      <c r="AI25"/>
+      <c r="AJ25"/>
+      <c r="AK25"/>
+      <c r="AL25"/>
+      <c r="AM25"/>
+      <c r="AN25"/>
+      <c r="AO25"/>
+      <c r="AP25"/>
+      <c r="AQ25"/>
+      <c r="AR25"/>
+      <c r="AS25"/>
+      <c r="AT25"/>
+      <c r="AU25"/>
+      <c r="AV25"/>
+      <c r="AW25"/>
+      <c r="AX25"/>
+      <c r="AY25"/>
+      <c r="AZ25"/>
+      <c r="BA25"/>
+      <c r="BB25"/>
+      <c r="BC25"/>
+      <c r="BD25"/>
+    </row>
+    <row r="26">
+      <c r="A26" t="s">
+        <v>83</v>
+      </c>
+      <c r="B26"/>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26"/>
+      <c r="K26"/>
+      <c r="L26"/>
+      <c r="M26"/>
+      <c r="N26"/>
+      <c r="O26"/>
+      <c r="P26"/>
+      <c r="Q26"/>
+      <c r="R26"/>
+      <c r="S26"/>
+      <c r="T26"/>
+      <c r="U26"/>
+      <c r="V26"/>
+      <c r="W26"/>
+      <c r="X26"/>
+      <c r="Y26"/>
+      <c r="Z26"/>
+      <c r="AA26"/>
+      <c r="AB26"/>
+      <c r="AC26"/>
+      <c r="AD26"/>
+      <c r="AE26"/>
+      <c r="AF26"/>
+      <c r="AG26"/>
+      <c r="AH26"/>
+      <c r="AI26"/>
+      <c r="AJ26"/>
+      <c r="AK26"/>
+      <c r="AL26"/>
+      <c r="AM26"/>
+      <c r="AN26"/>
+      <c r="AO26"/>
+      <c r="AP26"/>
+      <c r="AQ26"/>
+      <c r="AR26"/>
+      <c r="AS26"/>
+      <c r="AT26"/>
+      <c r="AU26"/>
+      <c r="AV26"/>
+      <c r="AW26"/>
+      <c r="AX26"/>
+      <c r="AY26"/>
+      <c r="AZ26"/>
+      <c r="BA26"/>
+      <c r="BB26"/>
+      <c r="BC26"/>
+      <c r="BD26"/>
+    </row>
+    <row r="27">
+      <c r="A27" t="s">
+        <v>83</v>
+      </c>
+      <c r="B27"/>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27"/>
+      <c r="K27"/>
+      <c r="L27"/>
+      <c r="M27"/>
+      <c r="N27"/>
+      <c r="O27"/>
+      <c r="P27"/>
+      <c r="Q27"/>
+      <c r="R27"/>
+      <c r="S27"/>
+      <c r="T27"/>
+      <c r="U27"/>
+      <c r="V27"/>
+      <c r="W27"/>
+      <c r="X27"/>
+      <c r="Y27"/>
+      <c r="Z27"/>
+      <c r="AA27"/>
+      <c r="AB27"/>
+      <c r="AC27"/>
+      <c r="AD27"/>
+      <c r="AE27"/>
+      <c r="AF27"/>
+      <c r="AG27"/>
+      <c r="AH27"/>
+      <c r="AI27"/>
+      <c r="AJ27"/>
+      <c r="AK27"/>
+      <c r="AL27"/>
+      <c r="AM27"/>
+      <c r="AN27"/>
+      <c r="AO27"/>
+      <c r="AP27"/>
+      <c r="AQ27"/>
+      <c r="AR27"/>
+      <c r="AS27"/>
+      <c r="AT27"/>
+      <c r="AU27"/>
+      <c r="AV27"/>
+      <c r="AW27"/>
+      <c r="AX27"/>
+      <c r="AY27"/>
+      <c r="AZ27"/>
+      <c r="BA27"/>
+      <c r="BB27"/>
+      <c r="BC27"/>
+      <c r="BD27"/>
+    </row>
+    <row r="28">
+      <c r="A28" t="s">
+        <v>83</v>
+      </c>
+      <c r="B28"/>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28"/>
+      <c r="K28"/>
+      <c r="L28"/>
+      <c r="M28"/>
+      <c r="N28"/>
+      <c r="O28"/>
+      <c r="P28"/>
+      <c r="Q28"/>
+      <c r="R28"/>
+      <c r="S28"/>
+      <c r="T28"/>
+      <c r="U28"/>
+      <c r="V28"/>
+      <c r="W28"/>
+      <c r="X28"/>
+      <c r="Y28"/>
+      <c r="Z28"/>
+      <c r="AA28"/>
+      <c r="AB28"/>
+      <c r="AC28"/>
+      <c r="AD28"/>
+      <c r="AE28"/>
+      <c r="AF28"/>
+      <c r="AG28"/>
+      <c r="AH28"/>
+      <c r="AI28"/>
+      <c r="AJ28"/>
+      <c r="AK28"/>
+      <c r="AL28"/>
+      <c r="AM28"/>
+      <c r="AN28"/>
+      <c r="AO28"/>
+      <c r="AP28"/>
+      <c r="AQ28"/>
+      <c r="AR28"/>
+      <c r="AS28"/>
+      <c r="AT28"/>
+      <c r="AU28"/>
+      <c r="AV28"/>
+      <c r="AW28"/>
+      <c r="AX28"/>
+      <c r="AY28"/>
+      <c r="AZ28"/>
+      <c r="BA28"/>
+      <c r="BB28"/>
+      <c r="BC28"/>
+      <c r="BD28"/>
+    </row>
+    <row r="29">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29"/>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29"/>
+      <c r="K29"/>
+      <c r="L29"/>
+      <c r="M29"/>
+      <c r="N29"/>
+      <c r="O29"/>
+      <c r="P29"/>
+      <c r="Q29"/>
+      <c r="R29"/>
+      <c r="S29"/>
+      <c r="T29"/>
+      <c r="U29"/>
+      <c r="V29"/>
+      <c r="W29"/>
+      <c r="X29"/>
+      <c r="Y29"/>
+      <c r="Z29"/>
+      <c r="AA29"/>
+      <c r="AB29"/>
+      <c r="AC29"/>
+      <c r="AD29"/>
+      <c r="AE29"/>
+      <c r="AF29"/>
+      <c r="AG29"/>
+      <c r="AH29"/>
+      <c r="AI29"/>
+      <c r="AJ29"/>
+      <c r="AK29"/>
+      <c r="AL29"/>
+      <c r="AM29"/>
+      <c r="AN29"/>
+      <c r="AO29"/>
+      <c r="AP29"/>
+      <c r="AQ29"/>
+      <c r="AR29"/>
+      <c r="AS29"/>
+      <c r="AT29"/>
+      <c r="AU29"/>
+      <c r="AV29"/>
+      <c r="AW29"/>
+      <c r="AX29"/>
+      <c r="AY29"/>
+      <c r="AZ29"/>
+      <c r="BA29"/>
+      <c r="BB29"/>
+      <c r="BC29"/>
+      <c r="BD29"/>
+    </row>
+    <row r="30">
+      <c r="A30" t="s">
+        <v>92</v>
+      </c>
+      <c r="B30"/>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30"/>
+      <c r="K30"/>
+      <c r="L30"/>
+      <c r="M30"/>
+      <c r="N30"/>
+      <c r="O30"/>
+      <c r="P30"/>
+      <c r="Q30"/>
+      <c r="R30"/>
+      <c r="S30"/>
+      <c r="T30"/>
+      <c r="U30"/>
+      <c r="V30"/>
+      <c r="W30"/>
+      <c r="X30"/>
+      <c r="Y30"/>
+      <c r="Z30"/>
+      <c r="AA30"/>
+      <c r="AB30"/>
+      <c r="AC30"/>
+      <c r="AD30"/>
+      <c r="AE30"/>
+      <c r="AF30"/>
+      <c r="AG30"/>
+      <c r="AH30"/>
+      <c r="AI30"/>
+      <c r="AJ30"/>
+      <c r="AK30"/>
+      <c r="AL30"/>
+      <c r="AM30"/>
+      <c r="AN30"/>
+      <c r="AO30"/>
+      <c r="AP30"/>
+      <c r="AQ30"/>
+      <c r="AR30"/>
+      <c r="AS30"/>
+      <c r="AT30"/>
+      <c r="AU30"/>
+      <c r="AV30"/>
+      <c r="AW30"/>
+      <c r="AX30"/>
+      <c r="AY30"/>
+      <c r="AZ30"/>
+      <c r="BA30"/>
+      <c r="BB30"/>
+      <c r="BC30"/>
+      <c r="BD30"/>
+    </row>
+    <row r="31">
+      <c r="A31" t="s">
+        <v>92</v>
+      </c>
+      <c r="B31"/>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31"/>
+      <c r="K31"/>
+      <c r="L31"/>
+      <c r="M31"/>
+      <c r="N31"/>
+      <c r="O31"/>
+      <c r="P31"/>
+      <c r="Q31"/>
+      <c r="R31"/>
+      <c r="S31"/>
+      <c r="T31"/>
+      <c r="U31"/>
+      <c r="V31"/>
+      <c r="W31"/>
+      <c r="X31"/>
+      <c r="Y31"/>
+      <c r="Z31"/>
+      <c r="AA31"/>
+      <c r="AB31"/>
+      <c r="AC31"/>
+      <c r="AD31"/>
+      <c r="AE31"/>
+      <c r="AF31"/>
+      <c r="AG31"/>
+      <c r="AH31"/>
+      <c r="AI31"/>
+      <c r="AJ31"/>
+      <c r="AK31"/>
+      <c r="AL31"/>
+      <c r="AM31"/>
+      <c r="AN31"/>
+      <c r="AO31"/>
+      <c r="AP31"/>
+      <c r="AQ31"/>
+      <c r="AR31"/>
+      <c r="AS31"/>
+      <c r="AT31"/>
+      <c r="AU31"/>
+      <c r="AV31"/>
+      <c r="AW31"/>
+      <c r="AX31"/>
+      <c r="AY31"/>
+      <c r="AZ31"/>
+      <c r="BA31"/>
+      <c r="BB31"/>
+      <c r="BC31"/>
+      <c r="BD31"/>
+    </row>
+    <row r="32">
+      <c r="A32" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32"/>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32"/>
+      <c r="K32"/>
+      <c r="L32"/>
+      <c r="M32"/>
+      <c r="N32"/>
+      <c r="O32"/>
+      <c r="P32"/>
+      <c r="Q32"/>
+      <c r="R32"/>
+      <c r="S32"/>
+      <c r="T32"/>
+      <c r="U32"/>
+      <c r="V32"/>
+      <c r="W32"/>
+      <c r="X32"/>
+      <c r="Y32"/>
+      <c r="Z32"/>
+      <c r="AA32"/>
+      <c r="AB32"/>
+      <c r="AC32"/>
+      <c r="AD32"/>
+      <c r="AE32"/>
+      <c r="AF32"/>
+      <c r="AG32"/>
+      <c r="AH32"/>
+      <c r="AI32"/>
+      <c r="AJ32"/>
+      <c r="AK32"/>
+      <c r="AL32"/>
+      <c r="AM32"/>
+      <c r="AN32"/>
+      <c r="AO32"/>
+      <c r="AP32"/>
+      <c r="AQ32"/>
+      <c r="AR32"/>
+      <c r="AS32"/>
+      <c r="AT32"/>
+      <c r="AU32"/>
+      <c r="AV32"/>
+      <c r="AW32"/>
+      <c r="AX32"/>
+      <c r="AY32"/>
+      <c r="AZ32"/>
+      <c r="BA32"/>
+      <c r="BB32"/>
+      <c r="BC32"/>
+      <c r="BD32"/>
+    </row>
+    <row r="33">
+      <c r="A33" t="s">
+        <v>82</v>
+      </c>
+      <c r="B33"/>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33"/>
+      <c r="K33"/>
+      <c r="L33"/>
+      <c r="M33"/>
+      <c r="N33"/>
+      <c r="O33"/>
+      <c r="P33"/>
+      <c r="Q33"/>
+      <c r="R33"/>
+      <c r="S33"/>
+      <c r="T33"/>
+      <c r="U33"/>
+      <c r="V33"/>
+      <c r="W33"/>
+      <c r="X33"/>
+      <c r="Y33"/>
+      <c r="Z33"/>
+      <c r="AA33"/>
+      <c r="AB33"/>
+      <c r="AC33"/>
+      <c r="AD33"/>
+      <c r="AE33"/>
+      <c r="AF33"/>
+      <c r="AG33"/>
+      <c r="AH33"/>
+      <c r="AI33"/>
+      <c r="AJ33"/>
+      <c r="AK33"/>
+      <c r="AL33"/>
+      <c r="AM33"/>
+      <c r="AN33"/>
+      <c r="AO33"/>
+      <c r="AP33"/>
+      <c r="AQ33"/>
+      <c r="AR33"/>
+      <c r="AS33"/>
+      <c r="AT33"/>
+      <c r="AU33"/>
+      <c r="AV33"/>
+      <c r="AW33"/>
+      <c r="AX33"/>
+      <c r="AY33"/>
+      <c r="AZ33"/>
+      <c r="BA33"/>
+      <c r="BB33"/>
+      <c r="BC33"/>
+      <c r="BD33"/>
+    </row>
+    <row r="34">
+      <c r="A34" t="s">
+        <v>82</v>
+      </c>
+      <c r="B34"/>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34"/>
+      <c r="K34"/>
+      <c r="L34"/>
+      <c r="M34"/>
+      <c r="N34"/>
+      <c r="O34"/>
+      <c r="P34"/>
+      <c r="Q34"/>
+      <c r="R34"/>
+      <c r="S34"/>
+      <c r="T34"/>
+      <c r="U34"/>
+      <c r="V34"/>
+      <c r="W34"/>
+      <c r="X34"/>
+      <c r="Y34"/>
+      <c r="Z34"/>
+      <c r="AA34"/>
+      <c r="AB34"/>
+      <c r="AC34"/>
+      <c r="AD34"/>
+      <c r="AE34"/>
+      <c r="AF34"/>
+      <c r="AG34"/>
+      <c r="AH34"/>
+      <c r="AI34"/>
+      <c r="AJ34"/>
+      <c r="AK34"/>
+      <c r="AL34"/>
+      <c r="AM34"/>
+      <c r="AN34"/>
+      <c r="AO34"/>
+      <c r="AP34"/>
+      <c r="AQ34"/>
+      <c r="AR34"/>
+      <c r="AS34"/>
+      <c r="AT34"/>
+      <c r="AU34"/>
+      <c r="AV34"/>
+      <c r="AW34"/>
+      <c r="AX34"/>
+      <c r="AY34"/>
+      <c r="AZ34"/>
+      <c r="BA34"/>
+      <c r="BB34"/>
+      <c r="BC34"/>
+      <c r="BD34"/>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
+        <v>93</v>
+      </c>
+      <c r="B35"/>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35"/>
+      <c r="K35"/>
+      <c r="L35"/>
+      <c r="M35"/>
+      <c r="N35"/>
+      <c r="O35"/>
+      <c r="P35"/>
+      <c r="Q35"/>
+      <c r="R35"/>
+      <c r="S35"/>
+      <c r="T35"/>
+      <c r="U35"/>
+      <c r="V35"/>
+      <c r="W35"/>
+      <c r="X35"/>
+      <c r="Y35"/>
+      <c r="Z35"/>
+      <c r="AA35"/>
+      <c r="AB35"/>
+      <c r="AC35"/>
+      <c r="AD35"/>
+      <c r="AE35"/>
+      <c r="AF35"/>
+      <c r="AG35"/>
+      <c r="AH35"/>
+      <c r="AI35"/>
+      <c r="AJ35"/>
+      <c r="AK35"/>
+      <c r="AL35"/>
+      <c r="AM35"/>
+      <c r="AN35"/>
+      <c r="AO35"/>
+      <c r="AP35"/>
+      <c r="AQ35"/>
+      <c r="AR35"/>
+      <c r="AS35"/>
+      <c r="AT35"/>
+      <c r="AU35"/>
+      <c r="AV35"/>
+      <c r="AW35"/>
+      <c r="AX35"/>
+      <c r="AY35"/>
+      <c r="AZ35"/>
+      <c r="BA35"/>
+      <c r="BB35"/>
+      <c r="BC35"/>
+      <c r="BD35"/>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
+        <v>93</v>
+      </c>
+      <c r="B36"/>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36"/>
+      <c r="K36"/>
+      <c r="L36"/>
+      <c r="M36"/>
+      <c r="N36"/>
+      <c r="O36"/>
+      <c r="P36"/>
+      <c r="Q36"/>
+      <c r="R36"/>
+      <c r="S36"/>
+      <c r="T36"/>
+      <c r="U36"/>
+      <c r="V36"/>
+      <c r="W36"/>
+      <c r="X36"/>
+      <c r="Y36"/>
+      <c r="Z36"/>
+      <c r="AA36"/>
+      <c r="AB36"/>
+      <c r="AC36"/>
+      <c r="AD36"/>
+      <c r="AE36"/>
+      <c r="AF36"/>
+      <c r="AG36"/>
+      <c r="AH36"/>
+      <c r="AI36"/>
+      <c r="AJ36"/>
+      <c r="AK36"/>
+      <c r="AL36"/>
+      <c r="AM36"/>
+      <c r="AN36"/>
+      <c r="AO36"/>
+      <c r="AP36"/>
+      <c r="AQ36"/>
+      <c r="AR36"/>
+      <c r="AS36"/>
+      <c r="AT36"/>
+      <c r="AU36"/>
+      <c r="AV36"/>
+      <c r="AW36"/>
+      <c r="AX36"/>
+      <c r="AY36"/>
+      <c r="AZ36"/>
+      <c r="BA36"/>
+      <c r="BB36"/>
+      <c r="BC36"/>
+      <c r="BD36"/>
+    </row>
+    <row r="37">
+      <c r="A37" t="s">
+        <v>93</v>
+      </c>
+      <c r="B37"/>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37"/>
+      <c r="K37"/>
+      <c r="L37"/>
+      <c r="M37"/>
+      <c r="N37"/>
+      <c r="O37"/>
+      <c r="P37"/>
+      <c r="Q37"/>
+      <c r="R37"/>
+      <c r="S37"/>
+      <c r="T37"/>
+      <c r="U37"/>
+      <c r="V37"/>
+      <c r="W37"/>
+      <c r="X37"/>
+      <c r="Y37"/>
+      <c r="Z37"/>
+      <c r="AA37"/>
+      <c r="AB37"/>
+      <c r="AC37"/>
+      <c r="AD37"/>
+      <c r="AE37"/>
+      <c r="AF37"/>
+      <c r="AG37"/>
+      <c r="AH37"/>
+      <c r="AI37"/>
+      <c r="AJ37"/>
+      <c r="AK37"/>
+      <c r="AL37"/>
+      <c r="AM37"/>
+      <c r="AN37"/>
+      <c r="AO37"/>
+      <c r="AP37"/>
+      <c r="AQ37"/>
+      <c r="AR37"/>
+      <c r="AS37"/>
+      <c r="AT37"/>
+      <c r="AU37"/>
+      <c r="AV37"/>
+      <c r="AW37"/>
+      <c r="AX37"/>
+      <c r="AY37"/>
+      <c r="AZ37"/>
+      <c r="BA37"/>
+      <c r="BB37"/>
+      <c r="BC37"/>
+      <c r="BD37"/>
+    </row>
+    <row r="38">
+      <c r="A38" t="s">
+        <v>85</v>
+      </c>
+      <c r="B38"/>
+      <c r="C38"/>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38"/>
+      <c r="K38"/>
+      <c r="L38"/>
+      <c r="M38"/>
+      <c r="N38"/>
+      <c r="O38"/>
+      <c r="P38"/>
+      <c r="Q38"/>
+      <c r="R38"/>
+      <c r="S38"/>
+      <c r="T38"/>
+      <c r="U38"/>
+      <c r="V38"/>
+      <c r="W38"/>
+      <c r="X38"/>
+      <c r="Y38"/>
+      <c r="Z38"/>
+      <c r="AA38"/>
+      <c r="AB38"/>
+      <c r="AC38"/>
+      <c r="AD38"/>
+      <c r="AE38"/>
+      <c r="AF38"/>
+      <c r="AG38"/>
+      <c r="AH38"/>
+      <c r="AI38"/>
+      <c r="AJ38"/>
+      <c r="AK38"/>
+      <c r="AL38"/>
+      <c r="AM38"/>
+      <c r="AN38"/>
+      <c r="AO38"/>
+      <c r="AP38"/>
+      <c r="AQ38"/>
+      <c r="AR38"/>
+      <c r="AS38"/>
+      <c r="AT38"/>
+      <c r="AU38"/>
+      <c r="AV38"/>
+      <c r="AW38"/>
+      <c r="AX38"/>
+      <c r="AY38"/>
+      <c r="AZ38"/>
+      <c r="BA38"/>
+      <c r="BB38"/>
+      <c r="BC38"/>
+      <c r="BD38"/>
+    </row>
+    <row r="39">
+      <c r="A39" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39"/>
+      <c r="C39"/>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39"/>
+      <c r="K39"/>
+      <c r="L39"/>
+      <c r="M39"/>
+      <c r="N39"/>
+      <c r="O39"/>
+      <c r="P39"/>
+      <c r="Q39"/>
+      <c r="R39"/>
+      <c r="S39"/>
+      <c r="T39"/>
+      <c r="U39"/>
+      <c r="V39"/>
+      <c r="W39"/>
+      <c r="X39"/>
+      <c r="Y39"/>
+      <c r="Z39"/>
+      <c r="AA39"/>
+      <c r="AB39"/>
+      <c r="AC39"/>
+      <c r="AD39"/>
+      <c r="AE39"/>
+      <c r="AF39"/>
+      <c r="AG39"/>
+      <c r="AH39"/>
+      <c r="AI39"/>
+      <c r="AJ39"/>
+      <c r="AK39"/>
+      <c r="AL39"/>
+      <c r="AM39"/>
+      <c r="AN39"/>
+      <c r="AO39"/>
+      <c r="AP39"/>
+      <c r="AQ39"/>
+      <c r="AR39"/>
+      <c r="AS39"/>
+      <c r="AT39"/>
+      <c r="AU39"/>
+      <c r="AV39"/>
+      <c r="AW39"/>
+      <c r="AX39"/>
+      <c r="AY39"/>
+      <c r="AZ39"/>
+      <c r="BA39"/>
+      <c r="BB39"/>
+      <c r="BC39"/>
+      <c r="BD39"/>
+    </row>
+    <row r="40">
+      <c r="A40" t="s">
+        <v>85</v>
+      </c>
+      <c r="B40"/>
+      <c r="C40"/>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40"/>
+      <c r="K40"/>
+      <c r="L40"/>
+      <c r="M40"/>
+      <c r="N40"/>
+      <c r="O40"/>
+      <c r="P40"/>
+      <c r="Q40"/>
+      <c r="R40"/>
+      <c r="S40"/>
+      <c r="T40"/>
+      <c r="U40"/>
+      <c r="V40"/>
+      <c r="W40"/>
+      <c r="X40"/>
+      <c r="Y40"/>
+      <c r="Z40"/>
+      <c r="AA40"/>
+      <c r="AB40"/>
+      <c r="AC40"/>
+      <c r="AD40"/>
+      <c r="AE40"/>
+      <c r="AF40"/>
+      <c r="AG40"/>
+      <c r="AH40"/>
+      <c r="AI40"/>
+      <c r="AJ40"/>
+      <c r="AK40"/>
+      <c r="AL40"/>
+      <c r="AM40"/>
+      <c r="AN40"/>
+      <c r="AO40"/>
+      <c r="AP40"/>
+      <c r="AQ40"/>
+      <c r="AR40"/>
+      <c r="AS40"/>
+      <c r="AT40"/>
+      <c r="AU40"/>
+      <c r="AV40"/>
+      <c r="AW40"/>
+      <c r="AX40"/>
+      <c r="AY40"/>
+      <c r="AZ40"/>
+      <c r="BA40"/>
+      <c r="BB40"/>
+      <c r="BC40"/>
+      <c r="BD40"/>
+    </row>
+    <row r="41">
+      <c r="A41" t="s">
+        <v>86</v>
+      </c>
+      <c r="B41"/>
+      <c r="C41"/>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41"/>
+      <c r="K41"/>
+      <c r="L41"/>
+      <c r="M41"/>
+      <c r="N41"/>
+      <c r="O41"/>
+      <c r="P41"/>
+      <c r="Q41"/>
+      <c r="R41"/>
+      <c r="S41"/>
+      <c r="T41"/>
+      <c r="U41"/>
+      <c r="V41"/>
+      <c r="W41"/>
+      <c r="X41"/>
+      <c r="Y41"/>
+      <c r="Z41"/>
+      <c r="AA41"/>
+      <c r="AB41"/>
+      <c r="AC41"/>
+      <c r="AD41"/>
+      <c r="AE41"/>
+      <c r="AF41"/>
+      <c r="AG41"/>
+      <c r="AH41"/>
+      <c r="AI41"/>
+      <c r="AJ41"/>
+      <c r="AK41"/>
+      <c r="AL41"/>
+      <c r="AM41"/>
+      <c r="AN41"/>
+      <c r="AO41"/>
+      <c r="AP41"/>
+      <c r="AQ41"/>
+      <c r="AR41"/>
+      <c r="AS41"/>
+      <c r="AT41"/>
+      <c r="AU41"/>
+      <c r="AV41"/>
+      <c r="AW41"/>
+      <c r="AX41"/>
+      <c r="AY41"/>
+      <c r="AZ41"/>
+      <c r="BA41"/>
+      <c r="BB41"/>
+      <c r="BC41"/>
+      <c r="BD41"/>
+    </row>
+    <row r="42">
+      <c r="A42" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42"/>
+      <c r="C42"/>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42"/>
+      <c r="K42"/>
+      <c r="L42"/>
+      <c r="M42"/>
+      <c r="N42"/>
+      <c r="O42"/>
+      <c r="P42"/>
+      <c r="Q42"/>
+      <c r="R42"/>
+      <c r="S42"/>
+      <c r="T42"/>
+      <c r="U42"/>
+      <c r="V42"/>
+      <c r="W42"/>
+      <c r="X42"/>
+      <c r="Y42"/>
+      <c r="Z42"/>
+      <c r="AA42"/>
+      <c r="AB42"/>
+      <c r="AC42"/>
+      <c r="AD42"/>
+      <c r="AE42"/>
+      <c r="AF42"/>
+      <c r="AG42"/>
+      <c r="AH42"/>
+      <c r="AI42"/>
+      <c r="AJ42"/>
+      <c r="AK42"/>
+      <c r="AL42"/>
+      <c r="AM42"/>
+      <c r="AN42"/>
+      <c r="AO42"/>
+      <c r="AP42"/>
+      <c r="AQ42"/>
+      <c r="AR42"/>
+      <c r="AS42"/>
+      <c r="AT42"/>
+      <c r="AU42"/>
+      <c r="AV42"/>
+      <c r="AW42"/>
+      <c r="AX42"/>
+      <c r="AY42"/>
+      <c r="AZ42"/>
+      <c r="BA42"/>
+      <c r="BB42"/>
+      <c r="BC42"/>
+      <c r="BD42"/>
+    </row>
+    <row r="43">
+      <c r="A43" t="s">
+        <v>86</v>
+      </c>
+      <c r="B43"/>
+      <c r="C43"/>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43"/>
+      <c r="K43"/>
+      <c r="L43"/>
+      <c r="M43"/>
+      <c r="N43"/>
+      <c r="O43"/>
+      <c r="P43"/>
+      <c r="Q43"/>
+      <c r="R43"/>
+      <c r="S43"/>
+      <c r="T43"/>
+      <c r="U43"/>
+      <c r="V43"/>
+      <c r="W43"/>
+      <c r="X43"/>
+      <c r="Y43"/>
+      <c r="Z43"/>
+      <c r="AA43"/>
+      <c r="AB43"/>
+      <c r="AC43"/>
+      <c r="AD43"/>
+      <c r="AE43"/>
+      <c r="AF43"/>
+      <c r="AG43"/>
+      <c r="AH43"/>
+      <c r="AI43"/>
+      <c r="AJ43"/>
+      <c r="AK43"/>
+      <c r="AL43"/>
+      <c r="AM43"/>
+      <c r="AN43"/>
+      <c r="AO43"/>
+      <c r="AP43"/>
+      <c r="AQ43"/>
+      <c r="AR43"/>
+      <c r="AS43"/>
+      <c r="AT43"/>
+      <c r="AU43"/>
+      <c r="AV43"/>
+      <c r="AW43"/>
+      <c r="AX43"/>
+      <c r="AY43"/>
+      <c r="AZ43"/>
+      <c r="BA43"/>
+      <c r="BB43"/>
+      <c r="BC43"/>
+      <c r="BD43"/>
+    </row>
+    <row r="44">
+      <c r="A44" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44"/>
+      <c r="C44"/>
+      <c r="D44"/>
+      <c r="E44"/>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44"/>
+      <c r="K44"/>
+      <c r="L44"/>
+      <c r="M44"/>
+      <c r="N44"/>
+      <c r="O44"/>
+      <c r="P44"/>
+      <c r="Q44"/>
+      <c r="R44"/>
+      <c r="S44"/>
+      <c r="T44"/>
+      <c r="U44"/>
+      <c r="V44"/>
+      <c r="W44"/>
+      <c r="X44"/>
+      <c r="Y44"/>
+      <c r="Z44"/>
+      <c r="AA44"/>
+      <c r="AB44"/>
+      <c r="AC44"/>
+      <c r="AD44"/>
+      <c r="AE44"/>
+      <c r="AF44"/>
+      <c r="AG44"/>
+      <c r="AH44"/>
+      <c r="AI44"/>
+      <c r="AJ44"/>
+      <c r="AK44"/>
+      <c r="AL44"/>
+      <c r="AM44"/>
+      <c r="AN44"/>
+      <c r="AO44"/>
+      <c r="AP44"/>
+      <c r="AQ44"/>
+      <c r="AR44"/>
+      <c r="AS44"/>
+      <c r="AT44"/>
+      <c r="AU44"/>
+      <c r="AV44"/>
+      <c r="AW44"/>
+      <c r="AX44"/>
+      <c r="AY44"/>
+      <c r="AZ44"/>
+      <c r="BA44"/>
+      <c r="BB44"/>
+      <c r="BC44"/>
+      <c r="BD44"/>
+    </row>
+    <row r="45">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45"/>
+      <c r="C45"/>
+      <c r="D45"/>
+      <c r="E45"/>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45"/>
+      <c r="K45"/>
+      <c r="L45"/>
+      <c r="M45"/>
+      <c r="N45"/>
+      <c r="O45"/>
+      <c r="P45"/>
+      <c r="Q45"/>
+      <c r="R45"/>
+      <c r="S45"/>
+      <c r="T45"/>
+      <c r="U45"/>
+      <c r="V45"/>
+      <c r="W45"/>
+      <c r="X45"/>
+      <c r="Y45"/>
+      <c r="Z45"/>
+      <c r="AA45"/>
+      <c r="AB45"/>
+      <c r="AC45"/>
+      <c r="AD45"/>
+      <c r="AE45"/>
+      <c r="AF45"/>
+      <c r="AG45"/>
+      <c r="AH45"/>
+      <c r="AI45"/>
+      <c r="AJ45"/>
+      <c r="AK45"/>
+      <c r="AL45"/>
+      <c r="AM45"/>
+      <c r="AN45"/>
+      <c r="AO45"/>
+      <c r="AP45"/>
+      <c r="AQ45"/>
+      <c r="AR45"/>
+      <c r="AS45"/>
+      <c r="AT45"/>
+      <c r="AU45"/>
+      <c r="AV45"/>
+      <c r="AW45"/>
+      <c r="AX45"/>
+      <c r="AY45"/>
+      <c r="AZ45"/>
+      <c r="BA45"/>
+      <c r="BB45"/>
+      <c r="BC45"/>
+      <c r="BD45"/>
+    </row>
+    <row r="46">
+      <c r="A46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B46"/>
+      <c r="C46"/>
+      <c r="D46"/>
+      <c r="E46"/>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46"/>
+      <c r="K46"/>
+      <c r="L46"/>
+      <c r="M46"/>
+      <c r="N46"/>
+      <c r="O46"/>
+      <c r="P46"/>
+      <c r="Q46"/>
+      <c r="R46"/>
+      <c r="S46"/>
+      <c r="T46"/>
+      <c r="U46"/>
+      <c r="V46"/>
+      <c r="W46"/>
+      <c r="X46"/>
+      <c r="Y46"/>
+      <c r="Z46"/>
+      <c r="AA46"/>
+      <c r="AB46"/>
+      <c r="AC46"/>
+      <c r="AD46"/>
+      <c r="AE46"/>
+      <c r="AF46"/>
+      <c r="AG46"/>
+      <c r="AH46"/>
+      <c r="AI46"/>
+      <c r="AJ46"/>
+      <c r="AK46"/>
+      <c r="AL46"/>
+      <c r="AM46"/>
+      <c r="AN46"/>
+      <c r="AO46"/>
+      <c r="AP46"/>
+      <c r="AQ46"/>
+      <c r="AR46"/>
+      <c r="AS46"/>
+      <c r="AT46"/>
+      <c r="AU46"/>
+      <c r="AV46"/>
+      <c r="AW46"/>
+      <c r="AX46"/>
+      <c r="AY46"/>
+      <c r="AZ46"/>
+      <c r="BA46"/>
+      <c r="BB46"/>
+      <c r="BC46"/>
+      <c r="BD46"/>
+    </row>
+    <row r="47">
+      <c r="A47" t="s">
+        <v>91</v>
+      </c>
+      <c r="B47"/>
+      <c r="C47"/>
+      <c r="D47"/>
+      <c r="E47"/>
+      <c r="F47"/>
+      <c r="G47"/>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47"/>
+      <c r="K47"/>
+      <c r="L47"/>
+      <c r="M47"/>
+      <c r="N47"/>
+      <c r="O47"/>
+      <c r="P47"/>
+      <c r="Q47"/>
+      <c r="R47"/>
+      <c r="S47"/>
+      <c r="T47"/>
+      <c r="U47"/>
+      <c r="V47"/>
+      <c r="W47"/>
+      <c r="X47"/>
+      <c r="Y47"/>
+      <c r="Z47"/>
+      <c r="AA47"/>
+      <c r="AB47"/>
+      <c r="AC47"/>
+      <c r="AD47"/>
+      <c r="AE47"/>
+      <c r="AF47"/>
+      <c r="AG47"/>
+      <c r="AH47"/>
+      <c r="AI47"/>
+      <c r="AJ47"/>
+      <c r="AK47"/>
+      <c r="AL47"/>
+      <c r="AM47"/>
+      <c r="AN47"/>
+      <c r="AO47"/>
+      <c r="AP47"/>
+      <c r="AQ47"/>
+      <c r="AR47"/>
+      <c r="AS47"/>
+      <c r="AT47"/>
+      <c r="AU47"/>
+      <c r="AV47"/>
+      <c r="AW47"/>
+      <c r="AX47"/>
+      <c r="AY47"/>
+      <c r="AZ47"/>
+      <c r="BA47"/>
+      <c r="BB47"/>
+      <c r="BC47"/>
+      <c r="BD47"/>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>91</v>
+      </c>
+      <c r="B48"/>
+      <c r="C48"/>
+      <c r="D48"/>
+      <c r="E48"/>
+      <c r="F48"/>
+      <c r="G48"/>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48"/>
+      <c r="K48"/>
+      <c r="L48"/>
+      <c r="M48"/>
+      <c r="N48"/>
+      <c r="O48"/>
+      <c r="P48"/>
+      <c r="Q48"/>
+      <c r="R48"/>
+      <c r="S48"/>
+      <c r="T48"/>
+      <c r="U48"/>
+      <c r="V48"/>
+      <c r="W48"/>
+      <c r="X48"/>
+      <c r="Y48"/>
+      <c r="Z48"/>
+      <c r="AA48"/>
+      <c r="AB48"/>
+      <c r="AC48"/>
+      <c r="AD48"/>
+      <c r="AE48"/>
+      <c r="AF48"/>
+      <c r="AG48"/>
+      <c r="AH48"/>
+      <c r="AI48"/>
+      <c r="AJ48"/>
+      <c r="AK48"/>
+      <c r="AL48"/>
+      <c r="AM48"/>
+      <c r="AN48"/>
+      <c r="AO48"/>
+      <c r="AP48"/>
+      <c r="AQ48"/>
+      <c r="AR48"/>
+      <c r="AS48"/>
+      <c r="AT48"/>
+      <c r="AU48"/>
+      <c r="AV48"/>
+      <c r="AW48"/>
+      <c r="AX48"/>
+      <c r="AY48"/>
+      <c r="AZ48"/>
+      <c r="BA48"/>
+      <c r="BB48"/>
+      <c r="BC48"/>
+      <c r="BD48"/>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>91</v>
+      </c>
+      <c r="B49"/>
+      <c r="C49"/>
+      <c r="D49"/>
+      <c r="E49"/>
+      <c r="F49"/>
+      <c r="G49"/>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49"/>
+      <c r="K49"/>
+      <c r="L49"/>
+      <c r="M49"/>
+      <c r="N49"/>
+      <c r="O49"/>
+      <c r="P49"/>
+      <c r="Q49"/>
+      <c r="R49"/>
+      <c r="S49"/>
+      <c r="T49"/>
+      <c r="U49"/>
+      <c r="V49"/>
+      <c r="W49"/>
+      <c r="X49"/>
+      <c r="Y49"/>
+      <c r="Z49"/>
+      <c r="AA49"/>
+      <c r="AB49"/>
+      <c r="AC49"/>
+      <c r="AD49"/>
+      <c r="AE49"/>
+      <c r="AF49"/>
+      <c r="AG49"/>
+      <c r="AH49"/>
+      <c r="AI49"/>
+      <c r="AJ49"/>
+      <c r="AK49"/>
+      <c r="AL49"/>
+      <c r="AM49"/>
+      <c r="AN49"/>
+      <c r="AO49"/>
+      <c r="AP49"/>
+      <c r="AQ49"/>
+      <c r="AR49"/>
+      <c r="AS49"/>
+      <c r="AT49"/>
+      <c r="AU49"/>
+      <c r="AV49"/>
+      <c r="AW49"/>
+      <c r="AX49"/>
+      <c r="AY49"/>
+      <c r="AZ49"/>
+      <c r="BA49"/>
+      <c r="BB49"/>
+      <c r="BC49"/>
+      <c r="BD49"/>
+    </row>
+    <row r="50">
+      <c r="A50" t="s">
+        <v>78</v>
+      </c>
+      <c r="B50"/>
+      <c r="C50"/>
+      <c r="D50"/>
+      <c r="E50"/>
+      <c r="F50"/>
+      <c r="G50"/>
+      <c r="H50"/>
+      <c r="I50"/>
+      <c r="J50"/>
+      <c r="K50"/>
+      <c r="L50"/>
+      <c r="M50"/>
+      <c r="N50"/>
+      <c r="O50"/>
+      <c r="P50"/>
+      <c r="Q50"/>
+      <c r="R50"/>
+      <c r="S50"/>
+      <c r="T50"/>
+      <c r="U50"/>
+      <c r="V50"/>
+      <c r="W50"/>
+      <c r="X50"/>
+      <c r="Y50"/>
+      <c r="Z50"/>
+      <c r="AA50"/>
+      <c r="AB50"/>
+      <c r="AC50"/>
+      <c r="AD50"/>
+      <c r="AE50"/>
+      <c r="AF50"/>
+      <c r="AG50"/>
+      <c r="AH50"/>
+      <c r="AI50"/>
+      <c r="AJ50"/>
+      <c r="AK50"/>
+      <c r="AL50"/>
+      <c r="AM50"/>
+      <c r="AN50"/>
+      <c r="AO50"/>
+      <c r="AP50"/>
+      <c r="AQ50"/>
+      <c r="AR50"/>
+      <c r="AS50"/>
+      <c r="AT50"/>
+      <c r="AU50"/>
+      <c r="AV50"/>
+      <c r="AW50"/>
+      <c r="AX50"/>
+      <c r="AY50"/>
+      <c r="AZ50"/>
+      <c r="BA50"/>
+      <c r="BB50"/>
+      <c r="BC50"/>
+      <c r="BD50"/>
+    </row>
+    <row r="51">
+      <c r="A51" t="s">
+        <v>78</v>
+      </c>
+      <c r="B51"/>
+      <c r="C51"/>
+      <c r="D51"/>
+      <c r="E51"/>
+      <c r="F51"/>
+      <c r="G51"/>
+      <c r="H51"/>
+      <c r="I51"/>
+      <c r="J51"/>
+      <c r="K51"/>
+      <c r="L51"/>
+      <c r="M51"/>
+      <c r="N51"/>
+      <c r="O51"/>
+      <c r="P51"/>
+      <c r="Q51"/>
+      <c r="R51"/>
+      <c r="S51"/>
+      <c r="T51"/>
+      <c r="U51"/>
+      <c r="V51"/>
+      <c r="W51"/>
+      <c r="X51"/>
+      <c r="Y51"/>
+      <c r="Z51"/>
+      <c r="AA51"/>
+      <c r="AB51"/>
+      <c r="AC51"/>
+      <c r="AD51"/>
+      <c r="AE51"/>
+      <c r="AF51"/>
+      <c r="AG51"/>
+      <c r="AH51"/>
+      <c r="AI51"/>
+      <c r="AJ51"/>
+      <c r="AK51"/>
+      <c r="AL51"/>
+      <c r="AM51"/>
+      <c r="AN51"/>
+      <c r="AO51"/>
+      <c r="AP51"/>
+      <c r="AQ51"/>
+      <c r="AR51"/>
+      <c r="AS51"/>
+      <c r="AT51"/>
+      <c r="AU51"/>
+      <c r="AV51"/>
+      <c r="AW51"/>
+      <c r="AX51"/>
+      <c r="AY51"/>
+      <c r="AZ51"/>
+      <c r="BA51"/>
+      <c r="BB51"/>
+      <c r="BC51"/>
+      <c r="BD51"/>
+    </row>
+    <row r="52">
+      <c r="A52" t="s">
+        <v>78</v>
+      </c>
+      <c r="B52"/>
+      <c r="C52"/>
+      <c r="D52"/>
+      <c r="E52"/>
+      <c r="F52"/>
+      <c r="G52"/>
+      <c r="H52"/>
+      <c r="I52"/>
+      <c r="J52"/>
+      <c r="K52"/>
+      <c r="L52"/>
+      <c r="M52"/>
+      <c r="N52"/>
+      <c r="O52"/>
+      <c r="P52"/>
+      <c r="Q52"/>
+      <c r="R52"/>
+      <c r="S52"/>
+      <c r="T52"/>
+      <c r="U52"/>
+      <c r="V52"/>
+      <c r="W52"/>
+      <c r="X52"/>
+      <c r="Y52"/>
+      <c r="Z52"/>
+      <c r="AA52"/>
+      <c r="AB52"/>
+      <c r="AC52"/>
+      <c r="AD52"/>
+      <c r="AE52"/>
+      <c r="AF52"/>
+      <c r="AG52"/>
+      <c r="AH52"/>
+      <c r="AI52"/>
+      <c r="AJ52"/>
+      <c r="AK52"/>
+      <c r="AL52"/>
+      <c r="AM52"/>
+      <c r="AN52"/>
+      <c r="AO52"/>
+      <c r="AP52"/>
+      <c r="AQ52"/>
+      <c r="AR52"/>
+      <c r="AS52"/>
+      <c r="AT52"/>
+      <c r="AU52"/>
+      <c r="AV52"/>
+      <c r="AW52"/>
+      <c r="AX52"/>
+      <c r="AY52"/>
+      <c r="AZ52"/>
+      <c r="BA52"/>
+      <c r="BB52"/>
+      <c r="BC52"/>
+      <c r="BD52"/>
+    </row>
+    <row r="53">
+      <c r="A53" t="s">
+        <v>80</v>
+      </c>
+      <c r="B53"/>
+      <c r="C53"/>
+      <c r="D53"/>
+      <c r="E53"/>
+      <c r="F53"/>
+      <c r="G53"/>
+      <c r="H53"/>
+      <c r="I53"/>
+      <c r="J53"/>
+      <c r="K53"/>
+      <c r="L53"/>
+      <c r="M53"/>
+      <c r="N53"/>
+      <c r="O53"/>
+      <c r="P53"/>
+      <c r="Q53"/>
+      <c r="R53"/>
+      <c r="S53"/>
+      <c r="T53"/>
+      <c r="U53"/>
+      <c r="V53"/>
+      <c r="W53"/>
+      <c r="X53"/>
+      <c r="Y53"/>
+      <c r="Z53"/>
+      <c r="AA53"/>
+      <c r="AB53"/>
+      <c r="AC53"/>
+      <c r="AD53"/>
+      <c r="AE53"/>
+      <c r="AF53"/>
+      <c r="AG53"/>
+      <c r="AH53"/>
+      <c r="AI53"/>
+      <c r="AJ53"/>
+      <c r="AK53"/>
+      <c r="AL53"/>
+      <c r="AM53"/>
+      <c r="AN53"/>
+      <c r="AO53"/>
+      <c r="AP53"/>
+      <c r="AQ53"/>
+      <c r="AR53"/>
+      <c r="AS53"/>
+      <c r="AT53"/>
+      <c r="AU53"/>
+      <c r="AV53"/>
+      <c r="AW53"/>
+      <c r="AX53"/>
+      <c r="AY53"/>
+      <c r="AZ53"/>
+      <c r="BA53"/>
+      <c r="BB53"/>
+      <c r="BC53"/>
+      <c r="BD53"/>
+    </row>
+    <row r="54">
+      <c r="A54" t="s">
+        <v>80</v>
+      </c>
+      <c r="B54"/>
+      <c r="C54"/>
+      <c r="D54"/>
+      <c r="E54"/>
+      <c r="F54"/>
+      <c r="G54"/>
+      <c r="H54"/>
+      <c r="I54"/>
+      <c r="J54"/>
+      <c r="K54"/>
+      <c r="L54"/>
+      <c r="M54"/>
+      <c r="N54"/>
+      <c r="O54"/>
+      <c r="P54"/>
+      <c r="Q54"/>
+      <c r="R54"/>
+      <c r="S54"/>
+      <c r="T54"/>
+      <c r="U54"/>
+      <c r="V54"/>
+      <c r="W54"/>
+      <c r="X54"/>
+      <c r="Y54"/>
+      <c r="Z54"/>
+      <c r="AA54"/>
+      <c r="AB54"/>
+      <c r="AC54"/>
+      <c r="AD54"/>
+      <c r="AE54"/>
+      <c r="AF54"/>
+      <c r="AG54"/>
+      <c r="AH54"/>
+      <c r="AI54"/>
+      <c r="AJ54"/>
+      <c r="AK54"/>
+      <c r="AL54"/>
+      <c r="AM54"/>
+      <c r="AN54"/>
+      <c r="AO54"/>
+      <c r="AP54"/>
+      <c r="AQ54"/>
+      <c r="AR54"/>
+      <c r="AS54"/>
+      <c r="AT54"/>
+      <c r="AU54"/>
+      <c r="AV54"/>
+      <c r="AW54"/>
+      <c r="AX54"/>
+      <c r="AY54"/>
+      <c r="AZ54"/>
+      <c r="BA54"/>
+      <c r="BB54"/>
+      <c r="BC54"/>
+      <c r="BD54"/>
+    </row>
+    <row r="55">
+      <c r="A55" t="s">
+        <v>80</v>
+      </c>
+      <c r="B55"/>
+      <c r="C55"/>
+      <c r="D55"/>
+      <c r="E55"/>
+      <c r="F55"/>
+      <c r="G55"/>
+      <c r="H55"/>
+      <c r="I55"/>
+      <c r="J55"/>
+      <c r="K55"/>
+      <c r="L55"/>
+      <c r="M55"/>
+      <c r="N55"/>
+      <c r="O55"/>
+      <c r="P55"/>
+      <c r="Q55"/>
+      <c r="R55"/>
+      <c r="S55"/>
+      <c r="T55"/>
+      <c r="U55"/>
+      <c r="V55"/>
+      <c r="W55"/>
+      <c r="X55"/>
+      <c r="Y55"/>
+      <c r="Z55"/>
+      <c r="AA55"/>
+      <c r="AB55"/>
+      <c r="AC55"/>
+      <c r="AD55"/>
+      <c r="AE55"/>
+      <c r="AF55"/>
+      <c r="AG55"/>
+      <c r="AH55"/>
+      <c r="AI55"/>
+      <c r="AJ55"/>
+      <c r="AK55"/>
+      <c r="AL55"/>
+      <c r="AM55"/>
+      <c r="AN55"/>
+      <c r="AO55"/>
+      <c r="AP55"/>
+      <c r="AQ55"/>
+      <c r="AR55"/>
+      <c r="AS55"/>
+      <c r="AT55"/>
+      <c r="AU55"/>
+      <c r="AV55"/>
+      <c r="AW55"/>
+      <c r="AX55"/>
+      <c r="AY55"/>
+      <c r="AZ55"/>
+      <c r="BA55"/>
+      <c r="BB55"/>
+      <c r="BC55"/>
+      <c r="BD55"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>